<commit_message>
update population in counties, municipalities
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BD49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -641,6 +641,774 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2">
+        <v>37697</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>35</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>32673</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>35545</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>40624</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>48</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>36835</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>149463</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>37</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>37525</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>35432</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>47</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>39745</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>49082</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>42220</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>32</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>39392</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>27</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>40620</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>38453</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>26</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>149448</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>33</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>32221</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>33873</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>33447</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>21</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>90208</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>39343</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>28</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>38235</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>24</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>95852</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>36</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>40623</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>40</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>39282</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>39818</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>14</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>1036991</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>22</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>196751</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>90240</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>43</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>32212</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>34</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>31946</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>40122</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>38611</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>31</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>148599</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>44</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>80814</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>38</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>1265711</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>23</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>31550</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>31574</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>45</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>71062</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>16</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>149462</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <v>15</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>64951</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>82166</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <v>39</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>1241002</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <v>46</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>38382</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <v>12</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>39528</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>31665</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <v>29</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>34704</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>37320</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <v>42</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>38202</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>49</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -648,7 +1416,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -659,6 +1427,11 @@
         <is>
           <t>id</t>
         </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>1267369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
top300 cities 2023 with flag
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD7"/>
+  <dimension ref="A1:BD1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -638,102 +638,6 @@
       <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>url_new</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>40620</v>
-      </c>
-      <c r="B2">
-        <v>20</v>
-      </c>
-      <c r="C2">
-        <v>22</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>33447</v>
-      </c>
-      <c r="B3">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>23</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>1036991</v>
-      </c>
-      <c r="B4">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>1265711</v>
-      </c>
-      <c r="B5">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>24</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>38235</v>
-      </c>
-      <c r="B6">
-        <v>24</v>
-      </c>
-      <c r="C6">
-        <v>25</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>64951</v>
-      </c>
-      <c r="B7">
-        <v>25</v>
-      </c>
-      <c r="C7">
-        <v>21</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>x1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update county list with flag
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD1"/>
+  <dimension ref="A1:BD32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -638,6 +638,502 @@
       <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>url_new</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>39282</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>31550</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>32221</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>32673</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>33873</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>35545</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>36835</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>37525</v>
+      </c>
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>38382</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>40122</v>
+      </c>
+      <c r="B11">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>18</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>39818</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>19</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>149462</v>
+      </c>
+      <c r="B13">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>7</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>71062</v>
+      </c>
+      <c r="B14">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>31946</v>
+      </c>
+      <c r="B15">
+        <v>17</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>90208</v>
+      </c>
+      <c r="B16">
+        <v>18</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>49082</v>
+      </c>
+      <c r="B17">
+        <v>19</v>
+      </c>
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>1036991</v>
+      </c>
+      <c r="B18">
+        <v>20</v>
+      </c>
+      <c r="C18">
+        <v>31</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>64951</v>
+      </c>
+      <c r="B19">
+        <v>21</v>
+      </c>
+      <c r="C19">
+        <v>34</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>40620</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>33447</v>
+      </c>
+      <c r="B21">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>21</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>1265711</v>
+      </c>
+      <c r="B22">
+        <v>24</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>38235</v>
+      </c>
+      <c r="B23">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>23</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>38453</v>
+      </c>
+      <c r="B24">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>24</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>39392</v>
+      </c>
+      <c r="B25">
+        <v>27</v>
+      </c>
+      <c r="C25">
+        <v>25</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>39343</v>
+      </c>
+      <c r="B26">
+        <v>28</v>
+      </c>
+      <c r="C26">
+        <v>26</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>31665</v>
+      </c>
+      <c r="B27">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>27</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>39745</v>
+      </c>
+      <c r="B28">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>28</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>38611</v>
+      </c>
+      <c r="B29">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>29</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>42220</v>
+      </c>
+      <c r="B30">
+        <v>32</v>
+      </c>
+      <c r="C30">
+        <v>30</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>149448</v>
+      </c>
+      <c r="B31">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>32</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>32212</v>
+      </c>
+      <c r="B32">
+        <v>34</v>
+      </c>
+      <c r="C32">
+        <v>33</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>x1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add some consolidated counties
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BD32"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -643,13 +643,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>39282</v>
+        <v>1036991</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -659,13 +659,13 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>31550</v>
+        <v>149448</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -675,13 +675,13 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>32221</v>
+        <v>32212</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C4">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -691,13 +691,13 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>32673</v>
+        <v>64951</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C5">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -707,431 +707,15 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>33873</v>
+        <v>37697</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="D6" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>35545</v>
-      </c>
-      <c r="B7">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>14</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>36835</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>15</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>37525</v>
-      </c>
-      <c r="B9">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>16</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>38382</v>
-      </c>
-      <c r="B10">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>17</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>40122</v>
-      </c>
-      <c r="B11">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>18</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>39818</v>
-      </c>
-      <c r="B12">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>19</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>149462</v>
-      </c>
-      <c r="B13">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>7</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>71062</v>
-      </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-      <c r="C14">
-        <v>8</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>31946</v>
-      </c>
-      <c r="B15">
-        <v>17</v>
-      </c>
-      <c r="C15">
-        <v>4</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>90208</v>
-      </c>
-      <c r="B16">
-        <v>18</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17">
-        <v>49082</v>
-      </c>
-      <c r="B17">
-        <v>19</v>
-      </c>
-      <c r="C17">
-        <v>6</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>1036991</v>
-      </c>
-      <c r="B18">
-        <v>20</v>
-      </c>
-      <c r="C18">
-        <v>31</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19">
-        <v>64951</v>
-      </c>
-      <c r="B19">
-        <v>21</v>
-      </c>
-      <c r="C19">
-        <v>34</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
-        <v>40620</v>
-      </c>
-      <c r="B20">
-        <v>22</v>
-      </c>
-      <c r="C20">
-        <v>20</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
-        <v>33447</v>
-      </c>
-      <c r="B21">
-        <v>23</v>
-      </c>
-      <c r="C21">
-        <v>21</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>1265711</v>
-      </c>
-      <c r="B22">
-        <v>24</v>
-      </c>
-      <c r="C22">
-        <v>22</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>38235</v>
-      </c>
-      <c r="B23">
-        <v>25</v>
-      </c>
-      <c r="C23">
-        <v>23</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>38453</v>
-      </c>
-      <c r="B24">
-        <v>26</v>
-      </c>
-      <c r="C24">
-        <v>24</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>39392</v>
-      </c>
-      <c r="B25">
-        <v>27</v>
-      </c>
-      <c r="C25">
-        <v>25</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>39343</v>
-      </c>
-      <c r="B26">
-        <v>28</v>
-      </c>
-      <c r="C26">
-        <v>26</v>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27">
-        <v>31665</v>
-      </c>
-      <c r="B27">
-        <v>29</v>
-      </c>
-      <c r="C27">
-        <v>27</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>39745</v>
-      </c>
-      <c r="B28">
-        <v>30</v>
-      </c>
-      <c r="C28">
-        <v>28</v>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>38611</v>
-      </c>
-      <c r="B29">
-        <v>31</v>
-      </c>
-      <c r="C29">
-        <v>29</v>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>42220</v>
-      </c>
-      <c r="B30">
-        <v>32</v>
-      </c>
-      <c r="C30">
-        <v>30</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>149448</v>
-      </c>
-      <c r="B31">
-        <v>33</v>
-      </c>
-      <c r="C31">
-        <v>32</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>32212</v>
-      </c>
-      <c r="B32">
-        <v>34</v>
-      </c>
-      <c r="C32">
-        <v>33</v>
-      </c>
-      <c r="D32" t="inlineStr">
         <is>
           <t>x1</t>
         </is>

</xml_diff>

<commit_message>
fix income 2023 in state entities
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB1"/>
+  <dimension ref="A1:BD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -622,12 +622,1002 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
+          <t>median_hh_income_old</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>median_hh_income_new</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
           <t>url_old</t>
         </is>
       </c>
-      <c r="BB1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>url_new</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <v>34704</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>27000</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>39528</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>53000</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>196751</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>18000</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>31946</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>08000</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>08</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>90208</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>21000</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>49082</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>05000</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>05</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>149462</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>25000</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>71062</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>15000</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>39282</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>49000</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>31550</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>01000</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>01</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>32221</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>32673</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>16000</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>33873</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>23000</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>35545</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>33000</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>36835</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>39000</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>37525</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>41000</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>38382</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>46000</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>40122</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>56000</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>39818</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>55000</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>1036991</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>19000</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>64951</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>30000</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>40620</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>37000</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>33447</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1265711</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>13000</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>38235</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>38453</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>47000</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>39392</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>51000</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>39343</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>50000</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>31665</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>06000</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>06</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>39745</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>54000</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>38611</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>48000</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>42220</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>36000</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>149448</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>09000</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>32212</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>37697</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>42000</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>95852</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>28000</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>149463</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>24000</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>80814</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>26000</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>82166</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>40623</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>04000</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>04</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>1267369</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>17000</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>37320</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>90240</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>22000</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>148599</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>29000</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>31574</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>02000</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>02</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>1241002</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>38000</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>35432</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>31000</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>40624</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>34000</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>38202</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>geo_id</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>44000</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>44</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing flags in school districts
</commit_message>
<xml_diff>
--- a/output/states_changes_report.xlsx
+++ b/output/states_changes_report.xlsx
@@ -353,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BF26"/>
+  <dimension ref="A1:BF8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -653,13 +653,13 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>39528</v>
+        <v>40620</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -669,13 +669,13 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>196751</v>
+        <v>33447</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -685,13 +685,13 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>31946</v>
+        <v>1265711</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -701,13 +701,13 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>90208</v>
+        <v>1036991</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -717,13 +717,13 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>49082</v>
+        <v>38235</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C6">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -733,13 +733,13 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>149462</v>
+        <v>38453</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -749,303 +749,15 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>71062</v>
+        <v>64951</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D8" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9">
-        <v>39282</v>
-      </c>
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10">
-        <v>31550</v>
-      </c>
-      <c r="B10">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11">
-        <v>32221</v>
-      </c>
-      <c r="B11">
-        <v>11</v>
-      </c>
-      <c r="C11">
-        <v>6</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12">
-        <v>32673</v>
-      </c>
-      <c r="B12">
-        <v>12</v>
-      </c>
-      <c r="C12">
-        <v>7</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13">
-        <v>33873</v>
-      </c>
-      <c r="B13">
-        <v>13</v>
-      </c>
-      <c r="C13">
-        <v>8</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14">
-        <v>35545</v>
-      </c>
-      <c r="B14">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>9</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15">
-        <v>36835</v>
-      </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
-      <c r="C15">
-        <v>10</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16">
-        <v>37525</v>
-      </c>
-      <c r="B16">
-        <v>16</v>
-      </c>
-      <c r="C16">
-        <v>11</v>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17">
-        <v>38382</v>
-      </c>
-      <c r="B17">
-        <v>17</v>
-      </c>
-      <c r="C17">
-        <v>12</v>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18">
-        <v>40122</v>
-      </c>
-      <c r="B18">
-        <v>18</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19">
-        <v>39818</v>
-      </c>
-      <c r="B19">
-        <v>19</v>
-      </c>
-      <c r="C19">
-        <v>14</v>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20">
-        <v>1036991</v>
-      </c>
-      <c r="B20">
-        <v>20</v>
-      </c>
-      <c r="C20">
-        <v>23</v>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21">
-        <v>64951</v>
-      </c>
-      <c r="B21">
-        <v>21</v>
-      </c>
-      <c r="C21">
-        <v>26</v>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>40620</v>
-      </c>
-      <c r="B22">
-        <v>22</v>
-      </c>
-      <c r="C22">
-        <v>20</v>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23">
-        <v>33447</v>
-      </c>
-      <c r="B23">
-        <v>23</v>
-      </c>
-      <c r="C23">
-        <v>21</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24">
-        <v>1265711</v>
-      </c>
-      <c r="B24">
-        <v>24</v>
-      </c>
-      <c r="C24">
-        <v>22</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25">
-        <v>38235</v>
-      </c>
-      <c r="B25">
-        <v>25</v>
-      </c>
-      <c r="C25">
-        <v>24</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>x1</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26">
-        <v>38453</v>
-      </c>
-      <c r="B26">
-        <v>26</v>
-      </c>
-      <c r="C26">
-        <v>25</v>
-      </c>
-      <c r="D26" t="inlineStr">
         <is>
           <t>x1</t>
         </is>

</xml_diff>